<commit_message>
Robin documentation and Bernhard updates
</commit_message>
<xml_diff>
--- a/Bernhard/BOM.xlsx
+++ b/Bernhard/BOM.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="269">
   <si>
     <t>Part</t>
   </si>
@@ -317,9 +317,6 @@
     <t>1/4-20 flange nut</t>
   </si>
   <si>
-    <t>9075A150</t>
-  </si>
-  <si>
     <t>1/4-28 flange nut</t>
   </si>
   <si>
@@ -437,9 +434,6 @@
     <t>Triple bracket, 90 degrees, 12 mount holes</t>
   </si>
   <si>
-    <t>Spring pin</t>
-  </si>
-  <si>
     <t>1x4 mm spring pin</t>
   </si>
   <si>
@@ -804,6 +798,33 @@
   </si>
   <si>
     <t>09/22/2011 01:54 AM （CST）</t>
+  </si>
+  <si>
+    <t>94100A110</t>
+  </si>
+  <si>
+    <t>94100A130</t>
+  </si>
+  <si>
+    <t>94100A140</t>
+  </si>
+  <si>
+    <t>91611A065</t>
+  </si>
+  <si>
+    <t>90759A150</t>
+  </si>
+  <si>
+    <t>10 bearings similar to R4A 2RS</t>
+  </si>
+  <si>
+    <t>Kit213</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>.250 (1/4) thick 3003-H14 Aluminum Plate</t>
   </si>
 </sst>
 </file>
@@ -814,7 +835,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -830,8 +851,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -850,6 +879,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -863,7 +898,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -875,6 +910,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1169,1441 +1209,1449 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
-      <c r="C1" t="s">
+    <row r="1" spans="3:7">
+      <c r="D1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="3:7">
+      <c r="C2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7">
+      <c r="C3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="2:6">
-      <c r="B2" t="s">
+    <row r="4" spans="3:7">
+      <c r="C4" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="B3" t="s">
+      <c r="D4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" t="s">
+      <c r="F4" t="s">
         <v>204</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>205</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="3:7">
+      <c r="C5" t="s">
         <v>206</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D5" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" t="s">
+      <c r="F5" t="s">
         <v>208</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>209</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" t="s">
         <v>210</v>
       </c>
-      <c r="F5" t="s">
+    </row>
+    <row r="7" spans="3:7">
+      <c r="C7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
-      <c r="B6" t="s">
+    <row r="8" spans="3:7">
+      <c r="C8" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
-      <c r="B8" t="s">
+    <row r="9" spans="3:7">
+      <c r="C9" t="s">
         <v>214</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
-      <c r="B9" t="s">
+    <row r="10" spans="3:7">
+      <c r="C10" t="s">
         <v>216</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>218</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>219</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="3:7">
+      <c r="C11" t="s">
         <v>220</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D11" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" t="s">
+        <v>208</v>
+      </c>
+      <c r="F11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7">
+      <c r="C12" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
-      <c r="B11" t="s">
+    <row r="13" spans="3:7">
+      <c r="C13" t="s">
         <v>222</v>
       </c>
-      <c r="C11" t="s">
-        <v>209</v>
-      </c>
-      <c r="D11" t="s">
-        <v>210</v>
-      </c>
-      <c r="E11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" t="s">
+      <c r="D13" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
-      <c r="B13" t="s">
+    <row r="14" spans="3:7">
+      <c r="C14" t="s">
         <v>224</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D14" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" t="s">
+      <c r="E14" t="s">
+        <v>227</v>
+      </c>
+      <c r="F14" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7">
+      <c r="C15" t="s">
         <v>226</v>
       </c>
-      <c r="C14" t="s">
-        <v>227</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="D15" s="6">
+        <v>41153</v>
+      </c>
+      <c r="E15" t="s">
         <v>229</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F15" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
-      <c r="B15" t="s">
-        <v>228</v>
-      </c>
-      <c r="C15" s="6">
-        <v>41153</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="16" spans="3:7">
+      <c r="C16" t="s">
         <v>231</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D16" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
-      <c r="B16" t="s">
+    <row r="17" spans="1:9">
+      <c r="C17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C16" s="6" t="s">
+    </row>
+    <row r="18" spans="1:9">
+      <c r="C18" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="B17" t="s">
-        <v>223</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="D18" s="7" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="B18" t="s">
+    <row r="19" spans="1:9">
+      <c r="C19" t="s">
         <v>236</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="B19" t="s">
-        <v>238</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="B20" t="s">
+    <row r="20" spans="1:9">
+      <c r="C20" t="s">
+        <v>256</v>
+      </c>
+      <c r="D20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E20" t="s">
         <v>258</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" t="s">
         <v>259</v>
       </c>
-      <c r="D20" t="s">
-        <v>260</v>
-      </c>
-      <c r="E20" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="C21" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" s="1">
-        <f>F21+'SDP-SI'!E1+'McMaster-Carr'!E1+VXB!E1+MetalsDepot!E1</f>
-        <v>813.22</v>
-      </c>
-      <c r="E21" t="s">
-        <v>111</v>
-      </c>
-      <c r="F21" s="1">
-        <f>F22+F40+F51+F61+F69+F83</f>
-        <v>542.72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+    </row>
+    <row r="21" spans="1:9">
+      <c r="D21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="1">
+        <f>G21+'SDP-SI'!E1+'McMaster-Carr'!E1+VXB!E1+MetalsDepot!E1</f>
+        <v>902.19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" s="1">
+        <f>G22+G40+G51+G61+G69+G83</f>
+        <v>574.72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="1">
-        <f>SUM(F24:F37)</f>
-        <v>197.31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="B23" s="2" t="s">
+      <c r="G22" s="1">
+        <f>SUM(G24:G37)</f>
+        <v>229.31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="C23" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" ref="G24:G36" si="0">E24*F24</f>
+        <v>18.239999999999998</v>
+      </c>
+      <c r="H24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" t="s">
         <v>152</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>9.1199999999999992</v>
-      </c>
-      <c r="F24" s="1">
-        <f t="shared" ref="F24:F36" si="0">D24*E24</f>
-        <v>18.239999999999998</v>
-      </c>
-      <c r="G24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>141</v>
-      </c>
-      <c r="B25" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1">
         <v>8</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
-      <c r="B26" t="s">
-        <v>155</v>
-      </c>
+    <row r="26" spans="1:9">
       <c r="C26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" t="s">
         <v>9</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>4</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <f t="shared" si="0"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
-      <c r="B27" t="s">
-        <v>156</v>
-      </c>
+    <row r="27" spans="1:9">
       <c r="C27" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" t="s">
         <v>11</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1">
-        <v>2</v>
+      <c r="E27">
+        <v>1</v>
       </c>
       <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="B28" t="s">
-        <v>157</v>
-      </c>
+    <row r="28" spans="1:9">
       <c r="C28" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" t="s">
         <v>13</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
         <v>1.37</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <f t="shared" si="0"/>
         <v>1.37</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="B29" t="s">
-        <v>158</v>
-      </c>
+    <row r="29" spans="1:9">
       <c r="C29" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" t="s">
         <v>14</v>
       </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="E29" s="1">
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
         <v>3.4</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <f t="shared" si="0"/>
         <v>6.8</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="B30" t="s">
-        <v>159</v>
-      </c>
+    <row r="30" spans="1:9">
       <c r="C30" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" t="s">
         <v>15</v>
       </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1">
         <v>7</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="B31" t="s">
-        <v>160</v>
-      </c>
+    <row r="31" spans="1:9">
       <c r="C31" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" t="s">
         <v>17</v>
       </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1">
         <v>2.8</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="B32" t="s">
-        <v>161</v>
-      </c>
+    <row r="32" spans="1:9">
       <c r="C32" t="s">
+        <v>159</v>
+      </c>
+      <c r="D32" t="s">
         <v>18</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>6</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>2.5</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="B33" s="9" t="s">
-        <v>162</v>
-      </c>
+    <row r="33" spans="1:8">
       <c r="C33" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="D33" s="9">
-        <v>1</v>
-      </c>
-      <c r="E33" s="10">
+        <v>160</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="E33" s="9">
+        <v>1</v>
+      </c>
+      <c r="F33" s="10">
         <v>28</v>
       </c>
-      <c r="F33" s="10">
+      <c r="G33" s="10">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="H33" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
-      <c r="B34" t="s">
-        <v>163</v>
-      </c>
+    <row r="34" spans="1:8">
       <c r="C34" t="s">
-        <v>257</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1">
+        <v>161</v>
+      </c>
+      <c r="D34" t="s">
+        <v>255</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
         <v>32.4</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <f t="shared" si="0"/>
         <v>32.4</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="B35" s="9" t="s">
-        <v>164</v>
-      </c>
+    <row r="35" spans="1:8">
       <c r="C35" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="D35" s="9">
-        <v>1</v>
-      </c>
-      <c r="E35" s="10">
+        <v>162</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10">
         <v>11.3</v>
       </c>
-      <c r="F35" s="10">
+      <c r="G35" s="10">
         <f t="shared" si="0"/>
         <v>11.3</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="H35" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
-      <c r="B36" s="9" t="s">
-        <v>165</v>
-      </c>
+    <row r="36" spans="1:8">
       <c r="C36" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="D36" s="9">
-        <v>1</v>
-      </c>
-      <c r="E36" s="10">
+        <v>163</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E36" s="14">
+        <v>2</v>
+      </c>
+      <c r="F36" s="10">
         <v>32</v>
       </c>
-      <c r="F36" s="10">
+      <c r="G36" s="10">
         <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="G36" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="B37" t="s">
-        <v>166</v>
-      </c>
+    <row r="37" spans="1:8">
       <c r="C37" t="s">
+        <v>164</v>
+      </c>
+      <c r="D37" t="s">
         <v>77</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="1">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
         <v>5.8</v>
       </c>
-      <c r="F37" s="1">
-        <f>D37*E37</f>
+      <c r="G37" s="1">
+        <f>E37*F37</f>
         <v>5.8</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="38" spans="1:8">
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>23</v>
       </c>
-      <c r="E40" t="s">
-        <v>112</v>
-      </c>
-      <c r="F40" s="1">
-        <f>SUM(F42:F50)</f>
+      <c r="F40" t="s">
+        <v>111</v>
+      </c>
+      <c r="G40" s="1">
+        <f>SUM(G42:G50)</f>
         <v>116.9</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
-      <c r="C41" s="2" t="s">
+    <row r="41" spans="1:8">
+      <c r="D41" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="E41" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
-      <c r="B42" t="s">
-        <v>167</v>
-      </c>
+    <row r="42" spans="1:8">
       <c r="C42" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" t="s">
         <v>24</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" s="1">
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1">
         <v>13.8</v>
       </c>
-      <c r="F42" s="1">
-        <f t="shared" ref="F42:F49" si="1">D42*E42</f>
+      <c r="G42" s="1">
+        <f t="shared" ref="G42:G49" si="1">E42*F42</f>
         <v>13.8</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="B43" t="s">
-        <v>168</v>
-      </c>
+    <row r="43" spans="1:8">
       <c r="C43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" t="s">
         <v>28</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>3</v>
       </c>
-      <c r="E43" s="1">
+      <c r="F43" s="1">
         <v>6</v>
       </c>
-      <c r="F43" s="1">
+      <c r="G43" s="1">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="B44" t="s">
-        <v>169</v>
-      </c>
+    <row r="44" spans="1:8">
       <c r="C44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" t="s">
         <v>30</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>3</v>
       </c>
-      <c r="E44" s="1">
+      <c r="F44" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F44" s="1">
+      <c r="G44" s="1">
         <f t="shared" si="1"/>
         <v>6.6000000000000005</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
-      <c r="B45" t="s">
-        <v>170</v>
-      </c>
+    <row r="45" spans="1:8">
       <c r="C45" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" t="s">
         <v>32</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" s="1">
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" s="1">
         <v>10.7</v>
       </c>
-      <c r="F45" s="1">
+      <c r="G45" s="1">
         <f t="shared" si="1"/>
         <v>10.7</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
-      <c r="B46" t="s">
-        <v>171</v>
-      </c>
+    <row r="46" spans="1:8">
       <c r="C46" t="s">
+        <v>169</v>
+      </c>
+      <c r="D46" t="s">
         <v>34</v>
       </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" s="1">
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1">
         <v>18.899999999999999</v>
       </c>
-      <c r="F46" s="1">
+      <c r="G46" s="1">
         <f t="shared" si="1"/>
         <v>18.899999999999999</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
-      <c r="B47" s="9" t="s">
-        <v>172</v>
-      </c>
+    <row r="47" spans="1:8">
       <c r="C47" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="D47" s="9">
-        <v>1</v>
-      </c>
-      <c r="E47" s="10">
+        <v>170</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1</v>
+      </c>
+      <c r="F47" s="10">
         <v>12.7</v>
       </c>
-      <c r="F47" s="10">
+      <c r="G47" s="10">
         <f t="shared" si="1"/>
         <v>12.7</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="H47" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
-      <c r="B48" s="9" t="s">
-        <v>173</v>
-      </c>
+    <row r="48" spans="1:8">
       <c r="C48" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="D48" s="9">
-        <v>2</v>
-      </c>
-      <c r="E48" s="10">
+        <v>171</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="E48" s="9">
+        <v>2</v>
+      </c>
+      <c r="F48" s="10">
         <v>12.4</v>
       </c>
-      <c r="F48" s="10">
+      <c r="G48" s="10">
         <f t="shared" si="1"/>
         <v>24.8</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="H48" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
-      <c r="B49" t="s">
-        <v>174</v>
-      </c>
+    <row r="49" spans="1:8">
       <c r="C49" t="s">
-        <v>256</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49" s="1">
+        <v>172</v>
+      </c>
+      <c r="D49" t="s">
+        <v>254</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
         <v>11.4</v>
       </c>
-      <c r="F49" s="1">
+      <c r="G49" s="1">
         <f t="shared" si="1"/>
         <v>11.4</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>36</v>
       </c>
-      <c r="E51" t="s">
-        <v>112</v>
-      </c>
-      <c r="F51" s="1">
-        <f>SUM(F53:F58)</f>
+      <c r="F51" t="s">
+        <v>111</v>
+      </c>
+      <c r="G51" s="1">
+        <f>SUM(G53:G58)</f>
         <v>43.8</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
-      <c r="C52" s="2" t="s">
+    <row r="52" spans="1:8">
+      <c r="D52" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="E52" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="H52" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
-      <c r="B53" t="s">
+    <row r="53" spans="1:8">
+      <c r="C53" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G53" s="1">
+        <f>E53*F53</f>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="H53" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="C54" t="s">
+        <v>174</v>
+      </c>
+      <c r="D54" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="G54" s="1">
+        <f>E54*F54</f>
+        <v>9.5</v>
+      </c>
+      <c r="H54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="C55" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C53" t="s">
-        <v>30</v>
-      </c>
-      <c r="D53">
-        <v>3</v>
-      </c>
-      <c r="E53" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F53" s="1">
-        <f>D53*E53</f>
-        <v>6.6000000000000005</v>
-      </c>
-      <c r="G53" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="B54" t="s">
+      <c r="D55" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E55" s="9">
+        <v>1</v>
+      </c>
+      <c r="F55" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="G55" s="10">
+        <f>E55*F55</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="C56" t="s">
         <v>176</v>
       </c>
-      <c r="C54" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="F54" s="1">
-        <f>D54*E54</f>
-        <v>9.5</v>
-      </c>
-      <c r="G54" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="B55" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D55" s="9">
-        <v>1</v>
-      </c>
-      <c r="E55" s="10">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="F55" s="10">
-        <f>D55*E55</f>
-        <v>20.399999999999999</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="B56" t="s">
-        <v>178</v>
-      </c>
-      <c r="C56" t="s">
-        <v>255</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56" s="1">
+      <c r="D56" t="s">
+        <v>253</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1">
         <v>7.3</v>
       </c>
-      <c r="F56" s="1">
-        <f>D56*E56</f>
+      <c r="G56" s="1">
+        <f>E56*F56</f>
         <v>7.3</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>82</v>
       </c>
-      <c r="E61" t="s">
-        <v>112</v>
-      </c>
-      <c r="F61" s="1">
-        <f>SUM(F63:F64)</f>
+      <c r="F61" t="s">
+        <v>111</v>
+      </c>
+      <c r="G61" s="1">
+        <f>SUM(G63:G64)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
-      <c r="C62" s="2" t="s">
+    <row r="62" spans="1:8">
+      <c r="D62" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="E62" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
-      <c r="B63" t="s">
-        <v>179</v>
-      </c>
+    <row r="63" spans="1:8">
       <c r="C63" t="s">
+        <v>177</v>
+      </c>
+      <c r="D63" t="s">
         <v>88</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>4</v>
       </c>
-      <c r="E63" s="1">
-        <v>1</v>
-      </c>
       <c r="F63" s="1">
-        <f>D63*E63</f>
+        <v>1</v>
+      </c>
+      <c r="G63" s="1">
+        <f>E63*F63</f>
         <v>4</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>46</v>
       </c>
-      <c r="E69" t="s">
-        <v>112</v>
-      </c>
-      <c r="F69" s="3">
-        <f>SUM(F71:F80)</f>
+      <c r="F69" t="s">
+        <v>111</v>
+      </c>
+      <c r="G69" s="3">
+        <f>SUM(G71:G80)</f>
         <v>121.92000000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
-      <c r="C70" s="2" t="s">
+    <row r="70" spans="1:8">
+      <c r="D70" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="E70" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="H70" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
-      <c r="B71" t="s">
-        <v>180</v>
-      </c>
+    <row r="71" spans="1:8">
       <c r="C71" t="s">
+        <v>178</v>
+      </c>
+      <c r="D71" t="s">
         <v>67</v>
       </c>
-      <c r="D71">
-        <v>2</v>
-      </c>
-      <c r="E71" s="3">
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71" s="3">
         <f>3.7+1.8</f>
         <v>5.5</v>
       </c>
-      <c r="F71" s="3">
-        <f>D71*E71</f>
+      <c r="G71" s="3">
+        <f>E71*F71</f>
         <v>11</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
-      <c r="B72" s="9" t="s">
+    <row r="72" spans="1:8">
+      <c r="C72" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E72" s="9">
+        <v>6</v>
+      </c>
+      <c r="F72" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G72" s="10">
+        <f>E72*F72</f>
+        <v>3</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="C73" t="s">
+        <v>180</v>
+      </c>
+      <c r="D73" t="s">
+        <v>49</v>
+      </c>
+      <c r="E73">
+        <v>4</v>
+      </c>
+      <c r="F73" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="G73" s="1">
+        <f>E73*F73</f>
+        <v>49.6</v>
+      </c>
+      <c r="H73" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="C74" t="s">
         <v>181</v>
       </c>
-      <c r="C72" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="D72" s="9">
-        <v>6</v>
-      </c>
-      <c r="E72" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="F72" s="10">
-        <f>D72*E72</f>
-        <v>3</v>
-      </c>
-      <c r="G72" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="B73" t="s">
-        <v>182</v>
-      </c>
-      <c r="C73" t="s">
-        <v>49</v>
-      </c>
-      <c r="D73">
-        <v>4</v>
-      </c>
-      <c r="E73" s="1">
-        <v>12.4</v>
-      </c>
-      <c r="F73" s="1">
-        <f>D73*E73</f>
-        <v>49.6</v>
-      </c>
-      <c r="G73" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="B74" t="s">
-        <v>183</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>50</v>
       </c>
-      <c r="D74">
-        <v>2</v>
-      </c>
-      <c r="E74" s="3">
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="F74" s="3">
         <f>3.45+3.2</f>
         <v>6.65</v>
       </c>
-      <c r="F74" s="1">
-        <f>D74*E74</f>
+      <c r="G74" s="1">
+        <f>E74*F74</f>
         <v>13.3</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
-      <c r="B75" t="s">
+    <row r="75" spans="1:8">
+      <c r="C75" t="s">
+        <v>182</v>
+      </c>
+      <c r="D75" t="s">
+        <v>52</v>
+      </c>
+      <c r="E75">
+        <v>4</v>
+      </c>
+      <c r="F75" s="1">
+        <v>2.86</v>
+      </c>
+      <c r="G75" s="1">
+        <f>E75*F75</f>
+        <v>11.44</v>
+      </c>
+      <c r="H75" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>139</v>
+      </c>
+      <c r="C76" t="s">
+        <v>183</v>
+      </c>
+      <c r="D76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="F76" s="3">
+        <v>7.06</v>
+      </c>
+      <c r="G76" s="1">
+        <f t="shared" ref="G76:G80" si="2">E76*F76</f>
+        <v>14.12</v>
+      </c>
+      <c r="H76" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>139</v>
+      </c>
+      <c r="C77" t="s">
         <v>184</v>
       </c>
-      <c r="C75" t="s">
-        <v>52</v>
-      </c>
-      <c r="D75">
-        <v>4</v>
-      </c>
-      <c r="E75" s="1">
-        <v>2.86</v>
-      </c>
-      <c r="F75" s="1">
-        <f>D75*E75</f>
-        <v>11.44</v>
-      </c>
-      <c r="G75" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" t="s">
-        <v>141</v>
-      </c>
-      <c r="B76" t="s">
-        <v>185</v>
-      </c>
-      <c r="C76" t="s">
-        <v>54</v>
-      </c>
-      <c r="D76">
-        <v>2</v>
-      </c>
-      <c r="E76" s="3">
-        <v>7.06</v>
-      </c>
-      <c r="F76" s="1">
-        <f t="shared" ref="F76:F80" si="2">D76*E76</f>
-        <v>14.12</v>
-      </c>
-      <c r="G76" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" t="s">
-        <v>141</v>
-      </c>
-      <c r="B77" t="s">
-        <v>186</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>55</v>
       </c>
-      <c r="D77">
-        <v>2</v>
-      </c>
-      <c r="E77" s="1">
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="F77" s="1">
         <v>3.85</v>
       </c>
-      <c r="F77" s="1">
+      <c r="G77" s="1">
         <f t="shared" si="2"/>
         <v>7.7</v>
       </c>
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
-      <c r="B78" t="s">
-        <v>187</v>
-      </c>
+    <row r="78" spans="1:8">
       <c r="C78" t="s">
+        <v>185</v>
+      </c>
+      <c r="D78" t="s">
         <v>56</v>
       </c>
-      <c r="D78">
-        <v>1</v>
-      </c>
-      <c r="E78" s="1">
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1">
         <v>0.68</v>
       </c>
-      <c r="F78" s="1">
+      <c r="G78" s="1">
         <f t="shared" si="2"/>
         <v>0.68</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
-      <c r="B79" t="s">
-        <v>188</v>
-      </c>
+    <row r="79" spans="1:8">
       <c r="C79" t="s">
+        <v>186</v>
+      </c>
+      <c r="D79" t="s">
         <v>58</v>
       </c>
-      <c r="D79">
-        <v>2</v>
-      </c>
-      <c r="E79" s="1">
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79" s="1">
         <v>2.35</v>
       </c>
-      <c r="F79" s="1">
+      <c r="G79" s="1">
         <f t="shared" si="2"/>
         <v>4.7</v>
       </c>
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
-      <c r="B80" t="s">
-        <v>189</v>
-      </c>
+    <row r="80" spans="1:8">
       <c r="C80" t="s">
-        <v>137</v>
-      </c>
-      <c r="D80">
-        <v>2</v>
-      </c>
-      <c r="E80" s="1">
+        <v>187</v>
+      </c>
+      <c r="D80" t="s">
+        <v>136</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80" s="1">
         <v>3.19</v>
       </c>
-      <c r="F80" s="1">
+      <c r="G80" s="1">
         <f t="shared" si="2"/>
         <v>6.38</v>
       </c>
-      <c r="G80" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="H80" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
         <v>60</v>
       </c>
-      <c r="E83" t="s">
-        <v>112</v>
-      </c>
-      <c r="F83" s="1">
-        <f>SUM(F85:F95)</f>
+      <c r="F83" t="s">
+        <v>111</v>
+      </c>
+      <c r="G83" s="1">
+        <f>SUM(G85:G95)</f>
         <v>58.79</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
-      <c r="C84" s="2" t="s">
+    <row r="84" spans="1:10">
+      <c r="D84" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="E84" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G84" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="H84" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="J84" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" t="s">
+        <v>139</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E85" s="9">
+        <v>1</v>
+      </c>
+      <c r="F85" s="10">
+        <v>18</v>
+      </c>
+      <c r="G85" s="10">
+        <f t="shared" ref="G85:G95" si="3">E85*F85</f>
+        <v>18</v>
+      </c>
+      <c r="H85" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J85" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" t="s">
+        <v>139</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D86" s="9" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="A85" t="s">
-        <v>141</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="D85" s="9">
-        <v>1</v>
-      </c>
-      <c r="E85" s="10">
-        <v>18</v>
-      </c>
-      <c r="F85" s="10">
-        <f t="shared" ref="F85:F95" si="3">D85*E85</f>
-        <v>18</v>
-      </c>
-      <c r="G85" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="I85" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" t="s">
-        <v>141</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="D86" s="9">
-        <v>1</v>
-      </c>
-      <c r="E86" s="10">
+      <c r="E86" s="9">
+        <v>1</v>
+      </c>
+      <c r="F86" s="10">
         <f>1.2*10.7</f>
         <v>12.839999999999998</v>
       </c>
-      <c r="F86" s="10">
+      <c r="G86" s="10">
         <f t="shared" si="3"/>
         <v>12.839999999999998</v>
       </c>
-      <c r="G86" s="9" t="s">
+      <c r="H86" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I86" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="B87" s="9" t="s">
-        <v>192</v>
-      </c>
+      <c r="J86" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="C87" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="D87" s="9">
-        <v>1</v>
-      </c>
-      <c r="E87" s="10">
+        <v>190</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E87" s="9">
+        <v>1</v>
+      </c>
+      <c r="F87" s="10">
         <v>6.5</v>
       </c>
-      <c r="F87" s="10">
+      <c r="G87" s="10">
         <f t="shared" si="3"/>
         <v>6.5</v>
       </c>
-      <c r="G87" s="9" t="s">
+      <c r="H87" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
-      <c r="B88" s="9" t="s">
-        <v>193</v>
-      </c>
+    <row r="88" spans="1:10">
       <c r="C88" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="D88" s="9">
-        <v>1</v>
-      </c>
-      <c r="E88" s="10">
+        <v>191</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="E88" s="9">
+        <v>1</v>
+      </c>
+      <c r="F88" s="10">
         <v>0.95</v>
       </c>
-      <c r="F88" s="10">
+      <c r="G88" s="10">
         <f t="shared" si="3"/>
         <v>0.95</v>
       </c>
-      <c r="G88" s="9" t="s">
+      <c r="H88" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
-      <c r="B89" t="s">
-        <v>194</v>
-      </c>
+    <row r="89" spans="1:10">
       <c r="C89" t="s">
+        <v>192</v>
+      </c>
+      <c r="D89" t="s">
         <v>73</v>
       </c>
-      <c r="D89">
-        <v>1</v>
-      </c>
-      <c r="E89" s="1">
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89" s="1">
         <v>1.4</v>
       </c>
-      <c r="F89" s="1">
+      <c r="G89" s="1">
         <f t="shared" si="3"/>
         <v>1.4</v>
       </c>
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
-      <c r="B90" s="9" t="s">
-        <v>195</v>
-      </c>
+    <row r="90" spans="1:10">
       <c r="C90" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D90" s="9">
-        <v>2</v>
-      </c>
-      <c r="E90" s="10">
+        <v>193</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="E90" s="9">
+        <v>2</v>
+      </c>
+      <c r="F90" s="10">
         <v>2.8</v>
       </c>
-      <c r="F90" s="10">
+      <c r="G90" s="10">
         <f t="shared" si="3"/>
         <v>5.6</v>
       </c>
-      <c r="G90" s="9" t="s">
+      <c r="H90" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
-      <c r="B91" t="s">
-        <v>196</v>
-      </c>
+    <row r="91" spans="1:10">
       <c r="C91" t="s">
-        <v>245</v>
-      </c>
-      <c r="D91">
-        <v>1</v>
-      </c>
-      <c r="E91" s="1">
+        <v>194</v>
+      </c>
+      <c r="D91" t="s">
+        <v>243</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F91" s="1">
+      <c r="G91" s="1">
         <f t="shared" si="3"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
-      <c r="B92" s="9" t="s">
-        <v>197</v>
-      </c>
+    <row r="92" spans="1:10">
       <c r="C92" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D92" s="9">
-        <v>1</v>
-      </c>
-      <c r="E92" s="10">
+        <v>195</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="E92" s="9">
+        <v>1</v>
+      </c>
+      <c r="F92" s="10">
         <v>0.7</v>
       </c>
-      <c r="F92" s="10">
+      <c r="G92" s="10">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="G92" s="9" t="s">
+      <c r="H92" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
-      <c r="B93" t="s">
-        <v>198</v>
-      </c>
+    <row r="93" spans="1:10">
       <c r="C93" t="s">
+        <v>196</v>
+      </c>
+      <c r="D93" t="s">
         <v>75</v>
       </c>
-      <c r="D93">
-        <v>2</v>
-      </c>
-      <c r="E93" s="1">
+      <c r="E93">
+        <v>2</v>
+      </c>
+      <c r="F93" s="1">
         <v>0.5</v>
       </c>
-      <c r="F93" s="1">
+      <c r="G93" s="1">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
-      <c r="B94" t="s">
-        <v>199</v>
-      </c>
+    <row r="94" spans="1:10">
       <c r="C94" t="s">
+        <v>197</v>
+      </c>
+      <c r="D94" t="s">
         <v>80</v>
       </c>
-      <c r="D94">
-        <v>2</v>
-      </c>
-      <c r="E94" s="1">
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94" s="1">
         <v>2.4</v>
       </c>
-      <c r="F94" s="1">
+      <c r="G94" s="1">
         <f t="shared" si="3"/>
         <v>4.8</v>
       </c>
-      <c r="G94" t="s">
+      <c r="H94" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
-      <c r="B95" t="s">
-        <v>200</v>
-      </c>
+    <row r="95" spans="1:10">
       <c r="C95" t="s">
+        <v>198</v>
+      </c>
+      <c r="D95" t="s">
         <v>81</v>
       </c>
-      <c r="D95">
-        <v>2</v>
-      </c>
-      <c r="E95" s="1">
+      <c r="E95">
+        <v>2</v>
+      </c>
+      <c r="F95" s="1">
         <v>2.4</v>
       </c>
-      <c r="F95" s="1">
+      <c r="G95" s="1">
         <f t="shared" si="3"/>
         <v>4.8</v>
       </c>
-      <c r="G95" t="s">
+      <c r="H95" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2618,7 +2666,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2628,11 +2676,11 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="D1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1">
         <f>E2</f>
-        <v>37.97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2640,11 +2688,11 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="1">
         <f>E4</f>
-        <v>37.97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2669,14 +2717,14 @@
         <v>26</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
         <v>37.97</v>
       </c>
       <c r="E4" s="1">
         <f>C4*D4</f>
-        <v>37.97</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
@@ -2691,8 +2739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="B41:F41"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2703,11 +2751,11 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="D1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1">
-        <f>E14+E21+E32+E4</f>
-        <v>85.76</v>
+        <f>E14+E21+E32+E4+E38</f>
+        <v>118.17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2722,11 +2770,11 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" s="1">
-        <f>SUM(E6:E7)</f>
-        <v>13.33</v>
+        <f>SUM(E6:E9)</f>
+        <v>38.72</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2748,7 +2796,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>139</v>
+        <v>263</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2761,26 +2809,61 @@
         <v>13.33</v>
       </c>
       <c r="F6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ref="E7:E9" si="0">C7*D7</f>
+        <v>6.05</v>
+      </c>
       <c r="F7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>9.1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>10.24</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>10.24</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="F8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="4" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2788,7 +2871,7 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" s="1">
         <f>SUM(E16:E17)</f>
@@ -2851,10 +2934,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E21" s="1">
         <f>SUM(E23:E30)</f>
@@ -2889,7 +2972,7 @@
         <v>7.65</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" ref="E23:E30" si="0">C23*D23</f>
+        <f t="shared" ref="E23:E30" si="1">C23*D23</f>
         <v>15.3</v>
       </c>
       <c r="F23" t="s">
@@ -2907,7 +2990,7 @@
         <v>1.18</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.18</v>
       </c>
       <c r="F24" t="s">
@@ -2925,7 +3008,7 @@
         <v>6.55</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.55</v>
       </c>
       <c r="F25" t="s">
@@ -2943,7 +3026,7 @@
         <v>3.07</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.07</v>
       </c>
       <c r="F26" t="s">
@@ -2961,7 +3044,7 @@
         <v>1.64</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.28</v>
       </c>
       <c r="F27" t="s">
@@ -2970,7 +3053,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="B28" t="s">
-        <v>99</v>
+        <v>264</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -2979,16 +3062,16 @@
         <v>1.64</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.28</v>
       </c>
       <c r="F28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="B29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2997,16 +3080,16 @@
         <v>2.72</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.72</v>
       </c>
       <c r="F29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="B30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -3015,11 +3098,11 @@
         <v>3.43</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.72</v>
       </c>
       <c r="F30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3031,7 +3114,7 @@
         <v>46</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E32" s="1">
         <f>SUM(E34:E36)</f>
@@ -3057,7 +3140,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="B34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3070,12 +3153,12 @@
         <v>12.32</v>
       </c>
       <c r="F34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3088,33 +3171,54 @@
         <v>4.29</v>
       </c>
       <c r="F35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="1">
+        <f>E40</f>
+        <v>7.02</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="D39" s="1"/>
+      <c r="B39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="40" spans="1:6">
       <c r="B40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" s="1">
         <v>3.51</v>
       </c>
       <c r="E40" s="1">
         <f>C40*D40</f>
-        <v>3.51</v>
+        <v>7.02</v>
       </c>
       <c r="F40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3129,29 +3233,44 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="D1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1">
-        <f>E5+SUM(E11:E13)+SUM(E17:E18)</f>
-        <v>74.349999999999994</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <f>SUM(E5:E7)+SUM(E11:E13)+SUM(E17:E18)</f>
+        <v>69.550000000000011</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="D2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" s="1">
+        <v>11.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="1">
+        <f>E1+E2</f>
+        <v>80.570000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -3168,9 +3287,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -3183,33 +3302,51 @@
         <v>14.850000000000001</v>
       </c>
       <c r="F5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="B6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="12">
         <v>4</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="13">
         <v>2.95</v>
       </c>
-      <c r="E6" s="1">
-        <f>C6*D6</f>
-        <v>11.8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>14.95</v>
+      </c>
+      <c r="E7" s="1">
+        <f>C7*D7</f>
+        <v>14.95</v>
+      </c>
+      <c r="F7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
@@ -3226,27 +3363,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="B11" t="s">
+    <row r="11" spans="1:7">
+      <c r="B11" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="12">
+        <v>5</v>
+      </c>
+      <c r="D11" s="13">
+        <v>2.95</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2.95</v>
-      </c>
-      <c r="E11" s="1">
-        <f>C11*D11</f>
-        <v>14.75</v>
-      </c>
-      <c r="F11" t="s">
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="B12" t="s">
-        <v>118</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3259,12 +3395,12 @@
         <v>5.95</v>
       </c>
       <c r="F12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -3277,15 +3413,15 @@
         <v>13.9</v>
       </c>
       <c r="F13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="B16" s="2" t="s">
         <v>0</v>
       </c>
@@ -3304,25 +3440,25 @@
     </row>
     <row r="17" spans="1:6">
       <c r="B17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="1">
-        <v>14.95</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="E17" s="1">
         <f>C17*D17</f>
-        <v>14.95</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="F17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3335,7 +3471,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="F18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3392,30 +3528,30 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="D1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1">
         <f>E2</f>
-        <v>72.42</v>
+        <v>139.75</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="1">
-        <f>SUM(E4:E7)</f>
-        <v>72.42</v>
+        <f>SUM(E4:E9)</f>
+        <v>139.75</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3437,7 +3573,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
@@ -3450,12 +3586,12 @@
         <v>22.98</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3464,16 +3600,16 @@
         <v>22.8</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E7" si="0">C5*D5</f>
+        <f t="shared" ref="E5:E8" si="0">C5*D5</f>
         <v>22.8</v>
       </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3486,12 +3622,12 @@
         <v>16.68</v>
       </c>
       <c r="F6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3504,14 +3640,36 @@
         <v>9.9600000000000009</v>
       </c>
       <c r="F7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" t="s">
         <v>131</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>22.45</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>22.45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E9" s="11">
+        <v>44.88</v>
+      </c>
       <c r="F9" s="2"/>
     </row>
     <row r="14" spans="1:6">

</xml_diff>